<commit_message>
Parse requirements.txt for python libraries
</commit_message>
<xml_diff>
--- a/tables/results/TableS4-Key-Resources-table.xlsx
+++ b/tables/results/TableS4-Key-Resources-table.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="949" uniqueCount="949">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="950" uniqueCount="950">
   <si>
     <t xml:space="preserve">R Package</t>
   </si>
@@ -2273,75 +2273,75 @@
     <t xml:space="preserve">Software</t>
   </si>
   <si>
+    <t xml:space="preserve">setuptools</t>
+  </si>
+  <si>
+    <t xml:space="preserve">46.3.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">six</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.14.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wheel </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.34.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">appdirs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">attrs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20.3.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">backcall</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bleach</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bx-python</t>
+  </si>
+  <si>
+    <t xml:space="preserve">certifi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020.12.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chardet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.0.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ConfigArgParse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CrossMap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.3.9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cycler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.10.0</t>
+  </si>
+  <si>
     <t xml:space="preserve">Cython</t>
   </si>
   <si>
     <t xml:space="preserve">0.29.15</t>
   </si>
   <si>
-    <t xml:space="preserve">setuptools</t>
-  </si>
-  <si>
-    <t xml:space="preserve">46.3.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">six</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.14.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wheel </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.34.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">appdirs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">attrs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20.3.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">backcall</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bleach</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bx-python</t>
-  </si>
-  <si>
-    <t xml:space="preserve">certifi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020.12.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">chardet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4.0.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ConfigArgParse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CrossMap</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.3.9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cycler</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.10.0</t>
-  </si>
-  <si>
     <t xml:space="preserve">datrie</t>
   </si>
   <si>
@@ -2381,6 +2381,9 @@
     <t xml:space="preserve">idna</t>
   </si>
   <si>
+    <t xml:space="preserve">2.10</t>
+  </si>
+  <si>
     <t xml:space="preserve">importlib-metadata</t>
   </si>
   <si>
@@ -2759,7 +2762,7 @@
     <t xml:space="preserve">0.9.3</t>
   </si>
   <si>
-    <t xml:space="preserve">strekla2</t>
+    <t xml:space="preserve">strelka2</t>
   </si>
   <si>
     <t xml:space="preserve">https://github.com/d3b-center/OpenPBTA-workflows/blob/master/cwl/kfdrc_strelka2_mutect2_manta_workflow.cwl; https://github.com/d3b-center/OpenPBTA-workflows/blob/master/cwl/kfdrc-mutect2_strelka2-wf.cwl</t>
@@ -6908,15 +6911,15 @@
         <v>758</v>
       </c>
       <c r="B5" t="s">
-        <v>759</v>
+        <v>213</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
+        <v>759</v>
+      </c>
+      <c r="B6" t="s">
         <v>760</v>
-      </c>
-      <c r="B6" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="7">
@@ -6924,31 +6927,31 @@
         <v>761</v>
       </c>
       <c r="B7" t="s">
-        <v>762</v>
+        <v>483</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="B8" t="s">
-        <v>483</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="B9" t="s">
-        <v>82</v>
+        <v>553</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
+        <v>764</v>
+      </c>
+      <c r="B10" t="s">
         <v>765</v>
-      </c>
-      <c r="B10" t="s">
-        <v>553</v>
       </c>
     </row>
     <row r="11">
@@ -6964,15 +6967,15 @@
         <v>768</v>
       </c>
       <c r="B12" t="s">
-        <v>769</v>
+        <v>445</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
+        <v>769</v>
+      </c>
+      <c r="B13" t="s">
         <v>770</v>
-      </c>
-      <c r="B13" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="14">
@@ -7052,12 +7055,12 @@
         <v>787</v>
       </c>
       <c r="B23" t="s">
-        <v>639</v>
+        <v>788</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="B24" t="s">
         <v>310</v>
@@ -7065,23 +7068,23 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="B25" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="B26" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="B27" t="s">
         <v>483</v>
@@ -7089,23 +7092,23 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="B28" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="B29" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="B30" t="s">
         <v>264</v>
@@ -7113,23 +7116,23 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="B31" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="B32" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="B33" t="s">
         <v>88</v>
@@ -7137,7 +7140,7 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="B34" t="s">
         <v>68</v>
@@ -7145,71 +7148,71 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="B35" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="B36" t="s">
-        <v>808</v>
+        <v>809</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="B37" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
       <c r="B38" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="B39" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="B40" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>817</v>
+        <v>818</v>
       </c>
       <c r="B41" t="s">
-        <v>818</v>
+        <v>819</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>819</v>
+        <v>820</v>
       </c>
       <c r="B42" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="B43" t="s">
         <v>82</v>
@@ -7217,15 +7220,15 @@
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>822</v>
+        <v>823</v>
       </c>
       <c r="B44" t="s">
-        <v>823</v>
+        <v>824</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
       <c r="B45" t="s">
         <v>224</v>
@@ -7233,7 +7236,7 @@
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c r="B46" t="s">
         <v>286</v>
@@ -7241,7 +7244,7 @@
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
       <c r="B47" t="s">
         <v>700</v>
@@ -7249,23 +7252,23 @@
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="B48" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="B49" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="B50" t="s">
         <v>306</v>
@@ -7273,47 +7276,47 @@
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="B51" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="B52" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="B53" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="B54" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c r="B55" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
       <c r="B56" t="s">
         <v>267</v>
@@ -7321,31 +7324,31 @@
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="B57" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="B58" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="B59" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="B60" t="s">
         <v>32</v>
@@ -7353,87 +7356,87 @@
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
       <c r="B61" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
       <c r="B62" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="B63" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
       <c r="B64" t="s">
-        <v>856</v>
+        <v>857</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="B65" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="B66" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="B67" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>863</v>
+        <v>864</v>
       </c>
       <c r="B68" t="s">
-        <v>864</v>
+        <v>865</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c r="B69" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c r="B70" t="s">
-        <v>868</v>
+        <v>869</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="B71" t="s">
         <v>332</v>
@@ -7441,7 +7444,7 @@
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c r="B72" t="s">
         <v>267</v>
@@ -7449,47 +7452,47 @@
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>871</v>
+        <v>872</v>
       </c>
       <c r="B73" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="B74" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="B75" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c r="B76" t="s">
-        <v>875</v>
+        <v>876</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>876</v>
+        <v>877</v>
       </c>
       <c r="B77" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>878</v>
+        <v>879</v>
       </c>
       <c r="B78" t="s">
         <v>171</v>
@@ -7497,7 +7500,7 @@
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>879</v>
+        <v>880</v>
       </c>
       <c r="B79" t="s">
         <v>443</v>
@@ -7505,23 +7508,23 @@
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>880</v>
+        <v>881</v>
       </c>
       <c r="B80" t="s">
-        <v>881</v>
+        <v>882</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>882</v>
+        <v>883</v>
       </c>
       <c r="B81" t="s">
-        <v>883</v>
+        <v>884</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="B82" t="s">
         <v>336</v>
@@ -7529,15 +7532,15 @@
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="B83" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="B84" t="s">
         <v>220</v>
@@ -7545,7 +7548,7 @@
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>888</v>
+        <v>889</v>
       </c>
       <c r="B85" t="s">
         <v>700</v>
@@ -7553,7 +7556,7 @@
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>889</v>
+        <v>890</v>
       </c>
       <c r="B86" t="s">
         <v>336</v>
@@ -7561,7 +7564,7 @@
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>890</v>
+        <v>891</v>
       </c>
       <c r="B87" t="s">
         <v>17</v>
@@ -7569,7 +7572,7 @@
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>891</v>
+        <v>892</v>
       </c>
       <c r="B88" t="s">
         <v>101</v>
@@ -7597,62 +7600,62 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>892</v>
+        <v>893</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>893</v>
+        <v>894</v>
       </c>
       <c r="B2" t="s">
-        <v>894</v>
+        <v>895</v>
       </c>
       <c r="C2" t="s">
-        <v>895</v>
+        <v>896</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>896</v>
+        <v>897</v>
       </c>
       <c r="B3" t="s">
-        <v>897</v>
+        <v>898</v>
       </c>
       <c r="C3" t="s">
-        <v>898</v>
+        <v>899</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>899</v>
+        <v>900</v>
       </c>
       <c r="B4" t="s">
-        <v>900</v>
+        <v>901</v>
       </c>
       <c r="C4" t="s">
-        <v>901</v>
+        <v>902</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>902</v>
+        <v>903</v>
       </c>
       <c r="B5" t="s">
-        <v>903</v>
+        <v>904</v>
       </c>
       <c r="C5" t="s">
-        <v>904</v>
+        <v>905</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>905</v>
+        <v>906</v>
       </c>
       <c r="B6" t="s">
-        <v>906</v>
+        <v>907</v>
       </c>
       <c r="C6" t="s">
-        <v>907</v>
+        <v>908</v>
       </c>
     </row>
   </sheetData>
@@ -7677,216 +7680,216 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>908</v>
+        <v>909</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>909</v>
+        <v>910</v>
       </c>
       <c r="B2" t="s">
-        <v>910</v>
+        <v>911</v>
       </c>
       <c r="C2" t="s">
-        <v>911</v>
+        <v>912</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>913</v>
+      </c>
+      <c r="B3" t="s">
+        <v>914</v>
+      </c>
+      <c r="C3" t="s">
         <v>912</v>
-      </c>
-      <c r="B3" t="s">
-        <v>913</v>
-      </c>
-      <c r="C3" t="s">
-        <v>911</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>914</v>
+        <v>915</v>
       </c>
       <c r="B4" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="C4" t="s">
-        <v>915</v>
+        <v>916</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
+        <v>917</v>
+      </c>
+      <c r="B5" t="s">
+        <v>918</v>
+      </c>
+      <c r="C5" t="s">
         <v>916</v>
-      </c>
-      <c r="B5" t="s">
-        <v>917</v>
-      </c>
-      <c r="C5" t="s">
-        <v>915</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>918</v>
+        <v>919</v>
       </c>
       <c r="B6" t="s">
         <v>75</v>
       </c>
       <c r="C6" t="s">
-        <v>919</v>
+        <v>920</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>920</v>
+        <v>921</v>
       </c>
       <c r="B7" t="s">
-        <v>921</v>
+        <v>922</v>
       </c>
       <c r="C7" t="s">
-        <v>922</v>
+        <v>923</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>923</v>
+        <v>924</v>
       </c>
       <c r="B8" t="s">
         <v>222</v>
       </c>
       <c r="C8" t="s">
-        <v>922</v>
+        <v>923</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>924</v>
+        <v>925</v>
       </c>
       <c r="B9" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="C9" t="s">
-        <v>922</v>
+        <v>923</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>925</v>
+        <v>926</v>
       </c>
       <c r="B10" t="s">
         <v>88</v>
       </c>
       <c r="C10" t="s">
-        <v>922</v>
+        <v>923</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="B11" t="s">
-        <v>927</v>
+        <v>928</v>
       </c>
       <c r="C11" t="s">
-        <v>928</v>
+        <v>929</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>929</v>
+        <v>930</v>
       </c>
       <c r="B12" t="s">
-        <v>930</v>
+        <v>931</v>
       </c>
       <c r="C12" t="s">
-        <v>931</v>
+        <v>932</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c r="B13" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
       <c r="C13" t="s">
-        <v>928</v>
+        <v>929</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>934</v>
+        <v>935</v>
       </c>
       <c r="B14" t="s">
         <v>38</v>
       </c>
       <c r="C14" t="s">
-        <v>935</v>
+        <v>936</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="B15" t="s">
         <v>68</v>
       </c>
       <c r="C15" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c r="B16" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
       <c r="C16" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>940</v>
+        <v>941</v>
       </c>
       <c r="B17" t="s">
-        <v>941</v>
+        <v>942</v>
       </c>
       <c r="C17" t="s">
-        <v>942</v>
+        <v>943</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
       <c r="B18" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="C18" t="s">
-        <v>945</v>
+        <v>946</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
       <c r="B19" t="s">
         <v>115</v>
       </c>
       <c r="C19" t="s">
-        <v>945</v>
+        <v>946</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>947</v>
+        <v>948</v>
       </c>
       <c r="B20" t="s">
-        <v>906</v>
+        <v>907</v>
       </c>
       <c r="C20" t="s">
-        <v>948</v>
+        <v>949</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add NGSCheckMate to S4
</commit_message>
<xml_diff>
--- a/tables/results/TableS4-Key-Resources-table.xlsx
+++ b/tables/results/TableS4-Key-Resources-table.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="950" uniqueCount="950">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="952" uniqueCount="952">
   <si>
     <t xml:space="preserve">R Package</t>
   </si>
@@ -2745,6 +2745,12 @@
   </si>
   <si>
     <t xml:space="preserve">Associated Workflow(s) or Script</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NGSCheckMate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/d3b-center/OpenPBTA-workflows/blob/master/cwl/bcf_call.cwl</t>
   </si>
   <si>
     <t xml:space="preserve">ControlFreeC</t>
@@ -7688,21 +7694,21 @@
         <v>910</v>
       </c>
       <c r="B2" t="s">
+        <v>325</v>
+      </c>
+      <c r="C2" t="s">
         <v>911</v>
-      </c>
-      <c r="C2" t="s">
-        <v>912</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>912</v>
+      </c>
+      <c r="B3" t="s">
         <v>913</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>914</v>
-      </c>
-      <c r="C3" t="s">
-        <v>912</v>
       </c>
     </row>
     <row r="4">
@@ -7710,10 +7716,10 @@
         <v>915</v>
       </c>
       <c r="B4" t="s">
-        <v>867</v>
+        <v>916</v>
       </c>
       <c r="C4" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
     </row>
     <row r="5">
@@ -7721,10 +7727,10 @@
         <v>917</v>
       </c>
       <c r="B5" t="s">
+        <v>867</v>
+      </c>
+      <c r="C5" t="s">
         <v>918</v>
-      </c>
-      <c r="C5" t="s">
-        <v>916</v>
       </c>
     </row>
     <row r="6">
@@ -7732,10 +7738,10 @@
         <v>919</v>
       </c>
       <c r="B6" t="s">
-        <v>75</v>
+        <v>920</v>
       </c>
       <c r="C6" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
     </row>
     <row r="7">
@@ -7743,76 +7749,76 @@
         <v>921</v>
       </c>
       <c r="B7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" t="s">
         <v>922</v>
-      </c>
-      <c r="C7" t="s">
-        <v>923</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
+        <v>923</v>
+      </c>
+      <c r="B8" t="s">
         <v>924</v>
       </c>
-      <c r="B8" t="s">
-        <v>222</v>
-      </c>
       <c r="C8" t="s">
-        <v>923</v>
+        <v>925</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
+        <v>926</v>
+      </c>
+      <c r="B9" t="s">
+        <v>222</v>
+      </c>
+      <c r="C9" t="s">
         <v>925</v>
-      </c>
-      <c r="B9" t="s">
-        <v>873</v>
-      </c>
-      <c r="C9" t="s">
-        <v>923</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="B10" t="s">
-        <v>88</v>
+        <v>873</v>
       </c>
       <c r="C10" t="s">
-        <v>923</v>
+        <v>925</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>927</v>
+        <v>928</v>
       </c>
       <c r="B11" t="s">
-        <v>928</v>
+        <v>88</v>
       </c>
       <c r="C11" t="s">
-        <v>929</v>
+        <v>925</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
+        <v>929</v>
+      </c>
+      <c r="B12" t="s">
         <v>930</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>931</v>
-      </c>
-      <c r="C12" t="s">
-        <v>932</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
+        <v>932</v>
+      </c>
+      <c r="B13" t="s">
         <v>933</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>934</v>
-      </c>
-      <c r="C13" t="s">
-        <v>929</v>
       </c>
     </row>
     <row r="14">
@@ -7820,10 +7826,10 @@
         <v>935</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>936</v>
       </c>
       <c r="C14" t="s">
-        <v>936</v>
+        <v>931</v>
       </c>
     </row>
     <row r="15">
@@ -7831,7 +7837,7 @@
         <v>937</v>
       </c>
       <c r="B15" t="s">
-        <v>68</v>
+        <v>38</v>
       </c>
       <c r="C15" t="s">
         <v>938</v>
@@ -7839,10 +7845,10 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>933</v>
+        <v>939</v>
       </c>
       <c r="B16" t="s">
-        <v>939</v>
+        <v>68</v>
       </c>
       <c r="C16" t="s">
         <v>940</v>
@@ -7850,46 +7856,57 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
+        <v>935</v>
+      </c>
+      <c r="B17" t="s">
         <v>941</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>942</v>
-      </c>
-      <c r="C17" t="s">
-        <v>943</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
+        <v>943</v>
+      </c>
+      <c r="B18" t="s">
         <v>944</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>945</v>
-      </c>
-      <c r="C18" t="s">
-        <v>946</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
+        <v>946</v>
+      </c>
+      <c r="B19" t="s">
         <v>947</v>
       </c>
-      <c r="B19" t="s">
-        <v>115</v>
-      </c>
       <c r="C19" t="s">
-        <v>946</v>
+        <v>948</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
+        <v>949</v>
+      </c>
+      <c r="B20" t="s">
+        <v>115</v>
+      </c>
+      <c r="C20" t="s">
         <v>948</v>
       </c>
-      <c r="B20" t="s">
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>950</v>
+      </c>
+      <c r="B21" t="s">
         <v>907</v>
       </c>
-      <c r="C20" t="s">
-        <v>949</v>
+      <c r="C21" t="s">
+        <v>951</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add NGSCheckMate to S4 (#1334)
Co-authored-by: Jaclyn Taroni <jaclyn.n.taroni@gmail.com>
</commit_message>
<xml_diff>
--- a/tables/results/TableS4-Key-Resources-table.xlsx
+++ b/tables/results/TableS4-Key-Resources-table.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="950" uniqueCount="950">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="952" uniqueCount="952">
   <si>
     <t xml:space="preserve">R Package</t>
   </si>
@@ -2745,6 +2745,12 @@
   </si>
   <si>
     <t xml:space="preserve">Associated Workflow(s) or Script</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NGSCheckMate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/d3b-center/OpenPBTA-workflows/blob/master/cwl/bcf_call.cwl</t>
   </si>
   <si>
     <t xml:space="preserve">ControlFreeC</t>
@@ -7688,21 +7694,21 @@
         <v>910</v>
       </c>
       <c r="B2" t="s">
+        <v>325</v>
+      </c>
+      <c r="C2" t="s">
         <v>911</v>
-      </c>
-      <c r="C2" t="s">
-        <v>912</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>912</v>
+      </c>
+      <c r="B3" t="s">
         <v>913</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>914</v>
-      </c>
-      <c r="C3" t="s">
-        <v>912</v>
       </c>
     </row>
     <row r="4">
@@ -7710,10 +7716,10 @@
         <v>915</v>
       </c>
       <c r="B4" t="s">
-        <v>867</v>
+        <v>916</v>
       </c>
       <c r="C4" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
     </row>
     <row r="5">
@@ -7721,10 +7727,10 @@
         <v>917</v>
       </c>
       <c r="B5" t="s">
+        <v>867</v>
+      </c>
+      <c r="C5" t="s">
         <v>918</v>
-      </c>
-      <c r="C5" t="s">
-        <v>916</v>
       </c>
     </row>
     <row r="6">
@@ -7732,10 +7738,10 @@
         <v>919</v>
       </c>
       <c r="B6" t="s">
-        <v>75</v>
+        <v>920</v>
       </c>
       <c r="C6" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
     </row>
     <row r="7">
@@ -7743,76 +7749,76 @@
         <v>921</v>
       </c>
       <c r="B7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" t="s">
         <v>922</v>
-      </c>
-      <c r="C7" t="s">
-        <v>923</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
+        <v>923</v>
+      </c>
+      <c r="B8" t="s">
         <v>924</v>
       </c>
-      <c r="B8" t="s">
-        <v>222</v>
-      </c>
       <c r="C8" t="s">
-        <v>923</v>
+        <v>925</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
+        <v>926</v>
+      </c>
+      <c r="B9" t="s">
+        <v>222</v>
+      </c>
+      <c r="C9" t="s">
         <v>925</v>
-      </c>
-      <c r="B9" t="s">
-        <v>873</v>
-      </c>
-      <c r="C9" t="s">
-        <v>923</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="B10" t="s">
-        <v>88</v>
+        <v>873</v>
       </c>
       <c r="C10" t="s">
-        <v>923</v>
+        <v>925</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>927</v>
+        <v>928</v>
       </c>
       <c r="B11" t="s">
-        <v>928</v>
+        <v>88</v>
       </c>
       <c r="C11" t="s">
-        <v>929</v>
+        <v>925</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
+        <v>929</v>
+      </c>
+      <c r="B12" t="s">
         <v>930</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>931</v>
-      </c>
-      <c r="C12" t="s">
-        <v>932</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
+        <v>932</v>
+      </c>
+      <c r="B13" t="s">
         <v>933</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>934</v>
-      </c>
-      <c r="C13" t="s">
-        <v>929</v>
       </c>
     </row>
     <row r="14">
@@ -7820,10 +7826,10 @@
         <v>935</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>936</v>
       </c>
       <c r="C14" t="s">
-        <v>936</v>
+        <v>931</v>
       </c>
     </row>
     <row r="15">
@@ -7831,7 +7837,7 @@
         <v>937</v>
       </c>
       <c r="B15" t="s">
-        <v>68</v>
+        <v>38</v>
       </c>
       <c r="C15" t="s">
         <v>938</v>
@@ -7839,10 +7845,10 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>933</v>
+        <v>939</v>
       </c>
       <c r="B16" t="s">
-        <v>939</v>
+        <v>68</v>
       </c>
       <c r="C16" t="s">
         <v>940</v>
@@ -7850,46 +7856,57 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
+        <v>935</v>
+      </c>
+      <c r="B17" t="s">
         <v>941</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>942</v>
-      </c>
-      <c r="C17" t="s">
-        <v>943</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
+        <v>943</v>
+      </c>
+      <c r="B18" t="s">
         <v>944</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>945</v>
-      </c>
-      <c r="C18" t="s">
-        <v>946</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
+        <v>946</v>
+      </c>
+      <c r="B19" t="s">
         <v>947</v>
       </c>
-      <c r="B19" t="s">
-        <v>115</v>
-      </c>
       <c r="C19" t="s">
-        <v>946</v>
+        <v>948</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
+        <v>949</v>
+      </c>
+      <c r="B20" t="s">
+        <v>115</v>
+      </c>
+      <c r="C20" t="s">
         <v>948</v>
       </c>
-      <c r="B20" t="s">
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>950</v>
+      </c>
+      <c r="B21" t="s">
         <v>907</v>
       </c>
-      <c r="C20" t="s">
-        <v>949</v>
+      <c r="C21" t="s">
+        <v>951</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add snippet about NBL - metastases
</commit_message>
<xml_diff>
--- a/tables/results/TableS4-Key-Resources-table.xlsx
+++ b/tables/results/TableS4-Key-Resources-table.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="950" uniqueCount="950">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="952" uniqueCount="952">
   <si>
     <t xml:space="preserve">R Package</t>
   </si>
@@ -2745,6 +2745,12 @@
   </si>
   <si>
     <t xml:space="preserve">Associated Workflow(s) or Script</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NGSCheckMate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/d3b-center/OpenPBTA-workflows/blob/master/cwl/bcf_call.cwl</t>
   </si>
   <si>
     <t xml:space="preserve">ControlFreeC</t>
@@ -7688,21 +7694,21 @@
         <v>910</v>
       </c>
       <c r="B2" t="s">
+        <v>325</v>
+      </c>
+      <c r="C2" t="s">
         <v>911</v>
-      </c>
-      <c r="C2" t="s">
-        <v>912</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>912</v>
+      </c>
+      <c r="B3" t="s">
         <v>913</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>914</v>
-      </c>
-      <c r="C3" t="s">
-        <v>912</v>
       </c>
     </row>
     <row r="4">
@@ -7710,10 +7716,10 @@
         <v>915</v>
       </c>
       <c r="B4" t="s">
-        <v>867</v>
+        <v>916</v>
       </c>
       <c r="C4" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
     </row>
     <row r="5">
@@ -7721,10 +7727,10 @@
         <v>917</v>
       </c>
       <c r="B5" t="s">
+        <v>867</v>
+      </c>
+      <c r="C5" t="s">
         <v>918</v>
-      </c>
-      <c r="C5" t="s">
-        <v>916</v>
       </c>
     </row>
     <row r="6">
@@ -7732,10 +7738,10 @@
         <v>919</v>
       </c>
       <c r="B6" t="s">
-        <v>75</v>
+        <v>920</v>
       </c>
       <c r="C6" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
     </row>
     <row r="7">
@@ -7743,76 +7749,76 @@
         <v>921</v>
       </c>
       <c r="B7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" t="s">
         <v>922</v>
-      </c>
-      <c r="C7" t="s">
-        <v>923</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
+        <v>923</v>
+      </c>
+      <c r="B8" t="s">
         <v>924</v>
       </c>
-      <c r="B8" t="s">
-        <v>222</v>
-      </c>
       <c r="C8" t="s">
-        <v>923</v>
+        <v>925</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
+        <v>926</v>
+      </c>
+      <c r="B9" t="s">
+        <v>222</v>
+      </c>
+      <c r="C9" t="s">
         <v>925</v>
-      </c>
-      <c r="B9" t="s">
-        <v>873</v>
-      </c>
-      <c r="C9" t="s">
-        <v>923</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="B10" t="s">
-        <v>88</v>
+        <v>873</v>
       </c>
       <c r="C10" t="s">
-        <v>923</v>
+        <v>925</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>927</v>
+        <v>928</v>
       </c>
       <c r="B11" t="s">
-        <v>928</v>
+        <v>88</v>
       </c>
       <c r="C11" t="s">
-        <v>929</v>
+        <v>925</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
+        <v>929</v>
+      </c>
+      <c r="B12" t="s">
         <v>930</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>931</v>
-      </c>
-      <c r="C12" t="s">
-        <v>932</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
+        <v>932</v>
+      </c>
+      <c r="B13" t="s">
         <v>933</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>934</v>
-      </c>
-      <c r="C13" t="s">
-        <v>929</v>
       </c>
     </row>
     <row r="14">
@@ -7820,10 +7826,10 @@
         <v>935</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>936</v>
       </c>
       <c r="C14" t="s">
-        <v>936</v>
+        <v>931</v>
       </c>
     </row>
     <row r="15">
@@ -7831,7 +7837,7 @@
         <v>937</v>
       </c>
       <c r="B15" t="s">
-        <v>68</v>
+        <v>38</v>
       </c>
       <c r="C15" t="s">
         <v>938</v>
@@ -7839,10 +7845,10 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>933</v>
+        <v>939</v>
       </c>
       <c r="B16" t="s">
-        <v>939</v>
+        <v>68</v>
       </c>
       <c r="C16" t="s">
         <v>940</v>
@@ -7850,46 +7856,57 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
+        <v>935</v>
+      </c>
+      <c r="B17" t="s">
         <v>941</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>942</v>
-      </c>
-      <c r="C17" t="s">
-        <v>943</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
+        <v>943</v>
+      </c>
+      <c r="B18" t="s">
         <v>944</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>945</v>
-      </c>
-      <c r="C18" t="s">
-        <v>946</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
+        <v>946</v>
+      </c>
+      <c r="B19" t="s">
         <v>947</v>
       </c>
-      <c r="B19" t="s">
-        <v>115</v>
-      </c>
       <c r="C19" t="s">
-        <v>946</v>
+        <v>948</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
+        <v>949</v>
+      </c>
+      <c r="B20" t="s">
+        <v>115</v>
+      </c>
+      <c r="C20" t="s">
         <v>948</v>
       </c>
-      <c r="B20" t="s">
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>950</v>
+      </c>
+      <c r="B21" t="s">
         <v>907</v>
       </c>
-      <c r="C20" t="s">
-        <v>949</v>
+      <c r="C21" t="s">
+        <v>951</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Re-ran tables to ensure all conflict issues are cleaned up and they are.
</commit_message>
<xml_diff>
--- a/tables/results/TableS4-Key-Resources-table.xlsx
+++ b/tables/results/TableS4-Key-Resources-table.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="952" uniqueCount="952">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="957" uniqueCount="957">
   <si>
     <t xml:space="preserve">R Package</t>
   </si>
@@ -611,6 +611,15 @@
     <t xml:space="preserve">1.0</t>
   </si>
   <si>
+    <t xml:space="preserve">extrafont</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">extrafontdb</t>
+  </si>
+  <si>
     <t xml:space="preserve">fansi</t>
   </si>
   <si>
@@ -1818,6 +1827,12 @@
   </si>
   <si>
     <t xml:space="preserve">0.15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rttf2pt1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.3.7</t>
   </si>
   <si>
     <t xml:space="preserve">rversions</t>
@@ -4039,7 +4054,7 @@
         <v>200</v>
       </c>
       <c r="B105" t="s">
-        <v>88</v>
+        <v>197</v>
       </c>
     </row>
     <row r="106">
@@ -4055,7 +4070,7 @@
         <v>203</v>
       </c>
       <c r="B107" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
     </row>
     <row r="108">
@@ -4071,7 +4086,7 @@
         <v>206</v>
       </c>
       <c r="B109" t="s">
-        <v>88</v>
+        <v>111</v>
       </c>
     </row>
     <row r="110">
@@ -4087,7 +4102,7 @@
         <v>209</v>
       </c>
       <c r="B111" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
     </row>
     <row r="112">
@@ -4095,23 +4110,23 @@
         <v>210</v>
       </c>
       <c r="B112" t="s">
-        <v>32</v>
+        <v>211</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B113" t="s">
-        <v>199</v>
+        <v>111</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B114" t="s">
-        <v>213</v>
+        <v>32</v>
       </c>
     </row>
     <row r="115">
@@ -4119,15 +4134,15 @@
         <v>214</v>
       </c>
       <c r="B115" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="s">
+        <v>215</v>
+      </c>
+      <c r="B116" t="s">
         <v>216</v>
-      </c>
-      <c r="B116" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="117">
@@ -4143,31 +4158,31 @@
         <v>219</v>
       </c>
       <c r="B118" t="s">
-        <v>220</v>
+        <v>115</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="s">
+        <v>220</v>
+      </c>
+      <c r="B119" t="s">
         <v>221</v>
-      </c>
-      <c r="B119" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="s">
+        <v>222</v>
+      </c>
+      <c r="B120" t="s">
         <v>223</v>
-      </c>
-      <c r="B120" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="s">
+        <v>224</v>
+      </c>
+      <c r="B121" t="s">
         <v>225</v>
-      </c>
-      <c r="B121" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="122">
@@ -4183,7 +4198,7 @@
         <v>228</v>
       </c>
       <c r="B123" t="s">
-        <v>15</v>
+        <v>153</v>
       </c>
     </row>
     <row r="124">
@@ -4199,15 +4214,15 @@
         <v>231</v>
       </c>
       <c r="B125" t="s">
-        <v>232</v>
+        <v>15</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="s">
+        <v>232</v>
+      </c>
+      <c r="B126" t="s">
         <v>233</v>
-      </c>
-      <c r="B126" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="127">
@@ -4223,23 +4238,23 @@
         <v>236</v>
       </c>
       <c r="B128" t="s">
-        <v>237</v>
+        <v>9</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="s">
+        <v>237</v>
+      </c>
+      <c r="B129" t="s">
         <v>238</v>
-      </c>
-      <c r="B129" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="s">
+        <v>239</v>
+      </c>
+      <c r="B130" t="s">
         <v>240</v>
-      </c>
-      <c r="B130" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="131">
@@ -4255,7 +4270,7 @@
         <v>243</v>
       </c>
       <c r="B132" t="s">
-        <v>149</v>
+        <v>240</v>
       </c>
     </row>
     <row r="133">
@@ -4271,31 +4286,31 @@
         <v>246</v>
       </c>
       <c r="B134" t="s">
-        <v>247</v>
+        <v>149</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="s">
+        <v>247</v>
+      </c>
+      <c r="B135" t="s">
         <v>248</v>
-      </c>
-      <c r="B135" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="s">
+        <v>249</v>
+      </c>
+      <c r="B136" t="s">
         <v>250</v>
-      </c>
-      <c r="B136" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="s">
+        <v>251</v>
+      </c>
+      <c r="B137" t="s">
         <v>252</v>
-      </c>
-      <c r="B137" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="138">
@@ -4311,47 +4326,47 @@
         <v>255</v>
       </c>
       <c r="B139" t="s">
-        <v>256</v>
+        <v>75</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="s">
+        <v>256</v>
+      </c>
+      <c r="B140" t="s">
         <v>257</v>
-      </c>
-      <c r="B140" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="s">
+        <v>258</v>
+      </c>
+      <c r="B141" t="s">
         <v>259</v>
-      </c>
-      <c r="B141" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="s">
+        <v>260</v>
+      </c>
+      <c r="B142" t="s">
         <v>261</v>
-      </c>
-      <c r="B142" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="s">
+        <v>262</v>
+      </c>
+      <c r="B143" t="s">
         <v>263</v>
-      </c>
-      <c r="B143" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="s">
+        <v>264</v>
+      </c>
+      <c r="B144" t="s">
         <v>265</v>
-      </c>
-      <c r="B144" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="145">
@@ -4367,39 +4382,39 @@
         <v>268</v>
       </c>
       <c r="B146" t="s">
-        <v>269</v>
+        <v>32</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="s">
+        <v>269</v>
+      </c>
+      <c r="B147" t="s">
         <v>270</v>
-      </c>
-      <c r="B147" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="s">
+        <v>271</v>
+      </c>
+      <c r="B148" t="s">
         <v>272</v>
-      </c>
-      <c r="B148" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="s">
+        <v>273</v>
+      </c>
+      <c r="B149" t="s">
         <v>274</v>
-      </c>
-      <c r="B149" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="s">
+        <v>275</v>
+      </c>
+      <c r="B150" t="s">
         <v>276</v>
-      </c>
-      <c r="B150" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="151">
@@ -4415,23 +4430,23 @@
         <v>279</v>
       </c>
       <c r="B152" t="s">
-        <v>280</v>
+        <v>153</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="s">
+        <v>280</v>
+      </c>
+      <c r="B153" t="s">
         <v>281</v>
-      </c>
-      <c r="B153" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="s">
+        <v>282</v>
+      </c>
+      <c r="B154" t="s">
         <v>283</v>
-      </c>
-      <c r="B154" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="155">
@@ -4439,15 +4454,15 @@
         <v>284</v>
       </c>
       <c r="B155" t="s">
-        <v>222</v>
+        <v>285</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B156" t="s">
-        <v>286</v>
+        <v>111</v>
       </c>
     </row>
     <row r="157">
@@ -4455,15 +4470,15 @@
         <v>287</v>
       </c>
       <c r="B157" t="s">
-        <v>288</v>
+        <v>225</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="s">
+        <v>288</v>
+      </c>
+      <c r="B158" t="s">
         <v>289</v>
-      </c>
-      <c r="B158" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="159">
@@ -4479,7 +4494,7 @@
         <v>292</v>
       </c>
       <c r="B160" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
     </row>
     <row r="161">
@@ -4495,39 +4510,39 @@
         <v>295</v>
       </c>
       <c r="B162" t="s">
-        <v>296</v>
+        <v>9</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="s">
+        <v>296</v>
+      </c>
+      <c r="B163" t="s">
         <v>297</v>
-      </c>
-      <c r="B163" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="s">
+        <v>298</v>
+      </c>
+      <c r="B164" t="s">
         <v>299</v>
-      </c>
-      <c r="B164" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="s">
+        <v>300</v>
+      </c>
+      <c r="B165" t="s">
         <v>301</v>
-      </c>
-      <c r="B165" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="s">
+        <v>302</v>
+      </c>
+      <c r="B166" t="s">
         <v>303</v>
-      </c>
-      <c r="B166" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="167">
@@ -4535,15 +4550,15 @@
         <v>304</v>
       </c>
       <c r="B167" t="s">
-        <v>254</v>
+        <v>305</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B168" t="s">
-        <v>306</v>
+        <v>11</v>
       </c>
     </row>
     <row r="169">
@@ -4551,55 +4566,55 @@
         <v>307</v>
       </c>
       <c r="B169" t="s">
-        <v>308</v>
+        <v>257</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="s">
+        <v>308</v>
+      </c>
+      <c r="B170" t="s">
         <v>309</v>
-      </c>
-      <c r="B170" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="s">
+        <v>310</v>
+      </c>
+      <c r="B171" t="s">
         <v>311</v>
-      </c>
-      <c r="B171" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="s">
+        <v>312</v>
+      </c>
+      <c r="B172" t="s">
         <v>313</v>
-      </c>
-      <c r="B172" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="s">
+        <v>314</v>
+      </c>
+      <c r="B173" t="s">
         <v>315</v>
-      </c>
-      <c r="B173" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="s">
+        <v>316</v>
+      </c>
+      <c r="B174" t="s">
         <v>317</v>
-      </c>
-      <c r="B174" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="s">
+        <v>318</v>
+      </c>
+      <c r="B175" t="s">
         <v>319</v>
-      </c>
-      <c r="B175" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="176">
@@ -4615,31 +4630,31 @@
         <v>322</v>
       </c>
       <c r="B177" t="s">
-        <v>323</v>
+        <v>42</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="s">
+        <v>323</v>
+      </c>
+      <c r="B178" t="s">
         <v>324</v>
-      </c>
-      <c r="B178" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="s">
+        <v>325</v>
+      </c>
+      <c r="B179" t="s">
         <v>326</v>
-      </c>
-      <c r="B179" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="s">
+        <v>327</v>
+      </c>
+      <c r="B180" t="s">
         <v>328</v>
-      </c>
-      <c r="B180" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="181">
@@ -4655,31 +4670,31 @@
         <v>331</v>
       </c>
       <c r="B182" t="s">
-        <v>332</v>
+        <v>75</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="s">
+        <v>332</v>
+      </c>
+      <c r="B183" t="s">
         <v>333</v>
-      </c>
-      <c r="B183" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="s">
+        <v>334</v>
+      </c>
+      <c r="B184" t="s">
         <v>335</v>
-      </c>
-      <c r="B184" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="s">
+        <v>336</v>
+      </c>
+      <c r="B185" t="s">
         <v>337</v>
-      </c>
-      <c r="B185" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="186">
@@ -4695,47 +4710,47 @@
         <v>340</v>
       </c>
       <c r="B187" t="s">
-        <v>341</v>
+        <v>111</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="s">
+        <v>341</v>
+      </c>
+      <c r="B188" t="s">
         <v>342</v>
-      </c>
-      <c r="B188" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="s">
+        <v>343</v>
+      </c>
+      <c r="B189" t="s">
         <v>344</v>
-      </c>
-      <c r="B189" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="s">
+        <v>345</v>
+      </c>
+      <c r="B190" t="s">
         <v>346</v>
-      </c>
-      <c r="B190" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="s">
+        <v>347</v>
+      </c>
+      <c r="B191" t="s">
         <v>348</v>
-      </c>
-      <c r="B191" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="s">
+        <v>349</v>
+      </c>
+      <c r="B192" t="s">
         <v>350</v>
-      </c>
-      <c r="B192" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="193">
@@ -4751,7 +4766,7 @@
         <v>353</v>
       </c>
       <c r="B194" t="s">
-        <v>222</v>
+        <v>101</v>
       </c>
     </row>
     <row r="195">
@@ -4767,47 +4782,47 @@
         <v>356</v>
       </c>
       <c r="B196" t="s">
-        <v>357</v>
+        <v>225</v>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="s">
+        <v>357</v>
+      </c>
+      <c r="B197" t="s">
         <v>358</v>
-      </c>
-      <c r="B197" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="s">
+        <v>359</v>
+      </c>
+      <c r="B198" t="s">
         <v>360</v>
-      </c>
-      <c r="B198" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="s">
+        <v>361</v>
+      </c>
+      <c r="B199" t="s">
         <v>362</v>
-      </c>
-      <c r="B199" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="s">
+        <v>363</v>
+      </c>
+      <c r="B200" t="s">
         <v>364</v>
-      </c>
-      <c r="B200" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="s">
+        <v>365</v>
+      </c>
+      <c r="B201" t="s">
         <v>366</v>
-      </c>
-      <c r="B201" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="202">
@@ -4823,23 +4838,23 @@
         <v>369</v>
       </c>
       <c r="B203" t="s">
-        <v>370</v>
+        <v>259</v>
       </c>
     </row>
     <row r="204">
       <c r="A204" t="s">
+        <v>370</v>
+      </c>
+      <c r="B204" t="s">
         <v>371</v>
-      </c>
-      <c r="B204" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="s">
+        <v>372</v>
+      </c>
+      <c r="B205" t="s">
         <v>373</v>
-      </c>
-      <c r="B205" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="206">
@@ -4855,7 +4870,7 @@
         <v>376</v>
       </c>
       <c r="B207" t="s">
-        <v>151</v>
+        <v>261</v>
       </c>
     </row>
     <row r="208">
@@ -4863,15 +4878,15 @@
         <v>377</v>
       </c>
       <c r="B208" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="B209" t="s">
-        <v>379</v>
+        <v>151</v>
       </c>
     </row>
     <row r="210">
@@ -4879,39 +4894,39 @@
         <v>380</v>
       </c>
       <c r="B210" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="s">
+        <v>381</v>
+      </c>
+      <c r="B211" t="s">
         <v>382</v>
-      </c>
-      <c r="B211" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="s">
+        <v>383</v>
+      </c>
+      <c r="B212" t="s">
         <v>384</v>
-      </c>
-      <c r="B212" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="s">
+        <v>385</v>
+      </c>
+      <c r="B213" t="s">
         <v>386</v>
-      </c>
-      <c r="B213" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="214">
       <c r="A214" t="s">
+        <v>387</v>
+      </c>
+      <c r="B214" t="s">
         <v>388</v>
-      </c>
-      <c r="B214" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="215">
@@ -4927,63 +4942,63 @@
         <v>391</v>
       </c>
       <c r="B216" t="s">
-        <v>392</v>
+        <v>105</v>
       </c>
     </row>
     <row r="217">
       <c r="A217" t="s">
+        <v>392</v>
+      </c>
+      <c r="B217" t="s">
         <v>393</v>
-      </c>
-      <c r="B217" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="218">
       <c r="A218" t="s">
+        <v>394</v>
+      </c>
+      <c r="B218" t="s">
         <v>395</v>
-      </c>
-      <c r="B218" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="219">
       <c r="A219" t="s">
+        <v>396</v>
+      </c>
+      <c r="B219" t="s">
         <v>397</v>
-      </c>
-      <c r="B219" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="220">
       <c r="A220" t="s">
+        <v>398</v>
+      </c>
+      <c r="B220" t="s">
         <v>399</v>
-      </c>
-      <c r="B220" t="s">
-        <v>400</v>
       </c>
     </row>
     <row r="221">
       <c r="A221" t="s">
+        <v>400</v>
+      </c>
+      <c r="B221" t="s">
         <v>401</v>
-      </c>
-      <c r="B221" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="222">
       <c r="A222" t="s">
+        <v>402</v>
+      </c>
+      <c r="B222" t="s">
         <v>403</v>
-      </c>
-      <c r="B222" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="223">
       <c r="A223" t="s">
+        <v>404</v>
+      </c>
+      <c r="B223" t="s">
         <v>405</v>
-      </c>
-      <c r="B223" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="224">
@@ -4999,31 +5014,31 @@
         <v>408</v>
       </c>
       <c r="B225" t="s">
-        <v>409</v>
+        <v>197</v>
       </c>
     </row>
     <row r="226">
       <c r="A226" t="s">
+        <v>409</v>
+      </c>
+      <c r="B226" t="s">
         <v>410</v>
-      </c>
-      <c r="B226" t="s">
-        <v>411</v>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="s">
+        <v>411</v>
+      </c>
+      <c r="B227" t="s">
         <v>412</v>
-      </c>
-      <c r="B227" t="s">
-        <v>413</v>
       </c>
     </row>
     <row r="228">
       <c r="A228" t="s">
+        <v>413</v>
+      </c>
+      <c r="B228" t="s">
         <v>414</v>
-      </c>
-      <c r="B228" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="229">
@@ -5031,23 +5046,23 @@
         <v>415</v>
       </c>
       <c r="B229" t="s">
-        <v>111</v>
+        <v>416</v>
       </c>
     </row>
     <row r="230">
       <c r="A230" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="B230" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
     </row>
     <row r="231">
       <c r="A231" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B231" t="s">
-        <v>418</v>
+        <v>111</v>
       </c>
     </row>
     <row r="232">
@@ -5055,15 +5070,15 @@
         <v>419</v>
       </c>
       <c r="B232" t="s">
-        <v>420</v>
+        <v>88</v>
       </c>
     </row>
     <row r="233">
       <c r="A233" t="s">
+        <v>420</v>
+      </c>
+      <c r="B233" t="s">
         <v>421</v>
-      </c>
-      <c r="B233" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="234">
@@ -5079,15 +5094,15 @@
         <v>424</v>
       </c>
       <c r="B235" t="s">
-        <v>425</v>
+        <v>173</v>
       </c>
     </row>
     <row r="236">
       <c r="A236" t="s">
+        <v>425</v>
+      </c>
+      <c r="B236" t="s">
         <v>426</v>
-      </c>
-      <c r="B236" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="237">
@@ -5103,15 +5118,15 @@
         <v>429</v>
       </c>
       <c r="B238" t="s">
-        <v>430</v>
+        <v>242</v>
       </c>
     </row>
     <row r="239">
       <c r="A239" t="s">
+        <v>430</v>
+      </c>
+      <c r="B239" t="s">
         <v>431</v>
-      </c>
-      <c r="B239" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="240">
@@ -5119,15 +5134,15 @@
         <v>432</v>
       </c>
       <c r="B240" t="s">
-        <v>271</v>
+        <v>433</v>
       </c>
     </row>
     <row r="241">
       <c r="A241" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="B241" t="s">
-        <v>434</v>
+        <v>151</v>
       </c>
     </row>
     <row r="242">
@@ -5135,15 +5150,15 @@
         <v>435</v>
       </c>
       <c r="B242" t="s">
-        <v>436</v>
+        <v>274</v>
       </c>
     </row>
     <row r="243">
       <c r="A243" t="s">
+        <v>436</v>
+      </c>
+      <c r="B243" t="s">
         <v>437</v>
-      </c>
-      <c r="B243" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="244">
@@ -5159,47 +5174,47 @@
         <v>440</v>
       </c>
       <c r="B245" t="s">
-        <v>441</v>
+        <v>301</v>
       </c>
     </row>
     <row r="246">
       <c r="A246" t="s">
+        <v>441</v>
+      </c>
+      <c r="B246" t="s">
         <v>442</v>
-      </c>
-      <c r="B246" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="247">
       <c r="A247" t="s">
+        <v>443</v>
+      </c>
+      <c r="B247" t="s">
         <v>444</v>
-      </c>
-      <c r="B247" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="248">
       <c r="A248" t="s">
+        <v>445</v>
+      </c>
+      <c r="B248" t="s">
         <v>446</v>
-      </c>
-      <c r="B248" t="s">
-        <v>447</v>
       </c>
     </row>
     <row r="249">
       <c r="A249" t="s">
+        <v>447</v>
+      </c>
+      <c r="B249" t="s">
         <v>448</v>
-      </c>
-      <c r="B249" t="s">
-        <v>449</v>
       </c>
     </row>
     <row r="250">
       <c r="A250" t="s">
+        <v>449</v>
+      </c>
+      <c r="B250" t="s">
         <v>450</v>
-      </c>
-      <c r="B250" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="251">
@@ -5215,7 +5230,7 @@
         <v>453</v>
       </c>
       <c r="B252" t="s">
-        <v>445</v>
+        <v>127</v>
       </c>
     </row>
     <row r="253">
@@ -5231,31 +5246,31 @@
         <v>456</v>
       </c>
       <c r="B254" t="s">
-        <v>457</v>
+        <v>448</v>
       </c>
     </row>
     <row r="255">
       <c r="A255" t="s">
+        <v>457</v>
+      </c>
+      <c r="B255" t="s">
         <v>458</v>
-      </c>
-      <c r="B255" t="s">
-        <v>459</v>
       </c>
     </row>
     <row r="256">
       <c r="A256" t="s">
+        <v>459</v>
+      </c>
+      <c r="B256" t="s">
         <v>460</v>
-      </c>
-      <c r="B256" t="s">
-        <v>461</v>
       </c>
     </row>
     <row r="257">
       <c r="A257" t="s">
+        <v>461</v>
+      </c>
+      <c r="B257" t="s">
         <v>462</v>
-      </c>
-      <c r="B257" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="258">
@@ -5263,31 +5278,31 @@
         <v>463</v>
       </c>
       <c r="B258" t="s">
-        <v>101</v>
+        <v>464</v>
       </c>
     </row>
     <row r="259">
       <c r="A259" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="B259" t="s">
-        <v>208</v>
+        <v>274</v>
       </c>
     </row>
     <row r="260">
       <c r="A260" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="B260" t="s">
-        <v>127</v>
+        <v>101</v>
       </c>
     </row>
     <row r="261">
       <c r="A261" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="B261" t="s">
-        <v>467</v>
+        <v>211</v>
       </c>
     </row>
     <row r="262">
@@ -5295,7 +5310,7 @@
         <v>468</v>
       </c>
       <c r="B262" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
     </row>
     <row r="263">
@@ -5303,15 +5318,15 @@
         <v>469</v>
       </c>
       <c r="B263" t="s">
-        <v>282</v>
+        <v>470</v>
       </c>
     </row>
     <row r="264">
       <c r="A264" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="B264" t="s">
-        <v>471</v>
+        <v>140</v>
       </c>
     </row>
     <row r="265">
@@ -5319,7 +5334,7 @@
         <v>472</v>
       </c>
       <c r="B265" t="s">
-        <v>383</v>
+        <v>285</v>
       </c>
     </row>
     <row r="266">
@@ -5327,23 +5342,23 @@
         <v>473</v>
       </c>
       <c r="B266" t="s">
-        <v>111</v>
+        <v>474</v>
       </c>
     </row>
     <row r="267">
       <c r="A267" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B267" t="s">
-        <v>151</v>
+        <v>386</v>
       </c>
     </row>
     <row r="268">
       <c r="A268" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="B268" t="s">
-        <v>476</v>
+        <v>111</v>
       </c>
     </row>
     <row r="269">
@@ -5351,23 +5366,23 @@
         <v>477</v>
       </c>
       <c r="B269" t="s">
-        <v>478</v>
+        <v>151</v>
       </c>
     </row>
     <row r="270">
       <c r="A270" t="s">
+        <v>478</v>
+      </c>
+      <c r="B270" t="s">
         <v>479</v>
-      </c>
-      <c r="B270" t="s">
-        <v>480</v>
       </c>
     </row>
     <row r="271">
       <c r="A271" t="s">
+        <v>480</v>
+      </c>
+      <c r="B271" t="s">
         <v>481</v>
-      </c>
-      <c r="B271" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="272">
@@ -5383,15 +5398,15 @@
         <v>484</v>
       </c>
       <c r="B273" t="s">
-        <v>485</v>
+        <v>111</v>
       </c>
     </row>
     <row r="274">
       <c r="A274" t="s">
+        <v>485</v>
+      </c>
+      <c r="B274" t="s">
         <v>486</v>
-      </c>
-      <c r="B274" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="275">
@@ -5407,15 +5422,15 @@
         <v>489</v>
       </c>
       <c r="B276" t="s">
-        <v>490</v>
+        <v>399</v>
       </c>
     </row>
     <row r="277">
       <c r="A277" t="s">
+        <v>490</v>
+      </c>
+      <c r="B277" t="s">
         <v>491</v>
-      </c>
-      <c r="B277" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="278">
@@ -5431,7 +5446,7 @@
         <v>494</v>
       </c>
       <c r="B279" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
     </row>
     <row r="280">
@@ -5439,23 +5454,23 @@
         <v>495</v>
       </c>
       <c r="B280" t="s">
-        <v>11</v>
+        <v>496</v>
       </c>
     </row>
     <row r="281">
       <c r="A281" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="B281" t="s">
-        <v>478</v>
+        <v>127</v>
       </c>
     </row>
     <row r="282">
       <c r="A282" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="B282" t="s">
-        <v>498</v>
+        <v>11</v>
       </c>
     </row>
     <row r="283">
@@ -5463,15 +5478,15 @@
         <v>499</v>
       </c>
       <c r="B283" t="s">
-        <v>500</v>
+        <v>481</v>
       </c>
     </row>
     <row r="284">
       <c r="A284" t="s">
+        <v>500</v>
+      </c>
+      <c r="B284" t="s">
         <v>501</v>
-      </c>
-      <c r="B284" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="285">
@@ -5479,15 +5494,15 @@
         <v>502</v>
       </c>
       <c r="B285" t="s">
-        <v>153</v>
+        <v>503</v>
       </c>
     </row>
     <row r="286">
       <c r="A286" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="B286" t="s">
-        <v>504</v>
+        <v>242</v>
       </c>
     </row>
     <row r="287">
@@ -5495,7 +5510,7 @@
         <v>505</v>
       </c>
       <c r="B287" t="s">
-        <v>476</v>
+        <v>153</v>
       </c>
     </row>
     <row r="288">
@@ -5511,7 +5526,7 @@
         <v>508</v>
       </c>
       <c r="B289" t="s">
-        <v>208</v>
+        <v>479</v>
       </c>
     </row>
     <row r="290">
@@ -5527,15 +5542,15 @@
         <v>511</v>
       </c>
       <c r="B291" t="s">
-        <v>512</v>
+        <v>211</v>
       </c>
     </row>
     <row r="292">
       <c r="A292" t="s">
+        <v>512</v>
+      </c>
+      <c r="B292" t="s">
         <v>513</v>
-      </c>
-      <c r="B292" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="293">
@@ -5551,23 +5566,23 @@
         <v>516</v>
       </c>
       <c r="B294" t="s">
-        <v>517</v>
+        <v>167</v>
       </c>
     </row>
     <row r="295">
       <c r="A295" t="s">
+        <v>517</v>
+      </c>
+      <c r="B295" t="s">
         <v>518</v>
-      </c>
-      <c r="B295" t="s">
-        <v>519</v>
       </c>
     </row>
     <row r="296">
       <c r="A296" t="s">
+        <v>519</v>
+      </c>
+      <c r="B296" t="s">
         <v>520</v>
-      </c>
-      <c r="B296" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="297">
@@ -5583,39 +5598,39 @@
         <v>523</v>
       </c>
       <c r="B298" t="s">
-        <v>524</v>
+        <v>342</v>
       </c>
     </row>
     <row r="299">
       <c r="A299" t="s">
+        <v>524</v>
+      </c>
+      <c r="B299" t="s">
         <v>525</v>
-      </c>
-      <c r="B299" t="s">
-        <v>526</v>
       </c>
     </row>
     <row r="300">
       <c r="A300" t="s">
+        <v>526</v>
+      </c>
+      <c r="B300" t="s">
         <v>527</v>
-      </c>
-      <c r="B300" t="s">
-        <v>528</v>
       </c>
     </row>
     <row r="301">
       <c r="A301" t="s">
+        <v>528</v>
+      </c>
+      <c r="B301" t="s">
         <v>529</v>
-      </c>
-      <c r="B301" t="s">
-        <v>530</v>
       </c>
     </row>
     <row r="302">
       <c r="A302" t="s">
+        <v>530</v>
+      </c>
+      <c r="B302" t="s">
         <v>531</v>
-      </c>
-      <c r="B302" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="303">
@@ -5631,31 +5646,31 @@
         <v>534</v>
       </c>
       <c r="B304" t="s">
-        <v>535</v>
+        <v>153</v>
       </c>
     </row>
     <row r="305">
       <c r="A305" t="s">
+        <v>535</v>
+      </c>
+      <c r="B305" t="s">
         <v>536</v>
-      </c>
-      <c r="B305" t="s">
-        <v>537</v>
       </c>
     </row>
     <row r="306">
       <c r="A306" t="s">
+        <v>537</v>
+      </c>
+      <c r="B306" t="s">
         <v>538</v>
-      </c>
-      <c r="B306" t="s">
-        <v>539</v>
       </c>
     </row>
     <row r="307">
       <c r="A307" t="s">
+        <v>539</v>
+      </c>
+      <c r="B307" t="s">
         <v>540</v>
-      </c>
-      <c r="B307" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="308">
@@ -5663,15 +5678,15 @@
         <v>541</v>
       </c>
       <c r="B308" t="s">
-        <v>222</v>
+        <v>542</v>
       </c>
     </row>
     <row r="309">
       <c r="A309" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="B309" t="s">
-        <v>543</v>
+        <v>225</v>
       </c>
     </row>
     <row r="310">
@@ -5679,7 +5694,7 @@
         <v>544</v>
       </c>
       <c r="B310" t="s">
-        <v>247</v>
+        <v>225</v>
       </c>
     </row>
     <row r="311">
@@ -5695,7 +5710,7 @@
         <v>547</v>
       </c>
       <c r="B312" t="s">
-        <v>153</v>
+        <v>250</v>
       </c>
     </row>
     <row r="313">
@@ -5711,7 +5726,7 @@
         <v>550</v>
       </c>
       <c r="B314" t="s">
-        <v>105</v>
+        <v>153</v>
       </c>
     </row>
     <row r="315">
@@ -5719,15 +5734,15 @@
         <v>551</v>
       </c>
       <c r="B315" t="s">
-        <v>306</v>
+        <v>552</v>
       </c>
     </row>
     <row r="316">
       <c r="A316" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="B316" t="s">
-        <v>553</v>
+        <v>105</v>
       </c>
     </row>
     <row r="317">
@@ -5735,7 +5750,7 @@
         <v>554</v>
       </c>
       <c r="B317" t="s">
-        <v>224</v>
+        <v>309</v>
       </c>
     </row>
     <row r="318">
@@ -5751,7 +5766,7 @@
         <v>557</v>
       </c>
       <c r="B319" t="s">
-        <v>282</v>
+        <v>227</v>
       </c>
     </row>
     <row r="320">
@@ -5767,15 +5782,15 @@
         <v>560</v>
       </c>
       <c r="B321" t="s">
-        <v>561</v>
+        <v>285</v>
       </c>
     </row>
     <row r="322">
       <c r="A322" t="s">
+        <v>561</v>
+      </c>
+      <c r="B322" t="s">
         <v>562</v>
-      </c>
-      <c r="B322" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="323">
@@ -5783,23 +5798,23 @@
         <v>563</v>
       </c>
       <c r="B323" t="s">
-        <v>68</v>
+        <v>564</v>
       </c>
     </row>
     <row r="324">
       <c r="A324" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="B324" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
     </row>
     <row r="325">
       <c r="A325" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="B325" t="s">
-        <v>566</v>
+        <v>68</v>
       </c>
     </row>
     <row r="326">
@@ -5807,15 +5822,15 @@
         <v>567</v>
       </c>
       <c r="B326" t="s">
-        <v>568</v>
+        <v>261</v>
       </c>
     </row>
     <row r="327">
       <c r="A327" t="s">
+        <v>568</v>
+      </c>
+      <c r="B327" t="s">
         <v>569</v>
-      </c>
-      <c r="B327" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="328">
@@ -5831,15 +5846,15 @@
         <v>572</v>
       </c>
       <c r="B329" t="s">
-        <v>573</v>
+        <v>202</v>
       </c>
     </row>
     <row r="330">
       <c r="A330" t="s">
+        <v>573</v>
+      </c>
+      <c r="B330" t="s">
         <v>574</v>
-      </c>
-      <c r="B330" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="331">
@@ -5855,63 +5870,63 @@
         <v>577</v>
       </c>
       <c r="B332" t="s">
-        <v>578</v>
+        <v>448</v>
       </c>
     </row>
     <row r="333">
       <c r="A333" t="s">
+        <v>578</v>
+      </c>
+      <c r="B333" t="s">
         <v>579</v>
-      </c>
-      <c r="B333" t="s">
-        <v>580</v>
       </c>
     </row>
     <row r="334">
       <c r="A334" t="s">
+        <v>580</v>
+      </c>
+      <c r="B334" t="s">
         <v>581</v>
-      </c>
-      <c r="B334" t="s">
-        <v>582</v>
       </c>
     </row>
     <row r="335">
       <c r="A335" t="s">
+        <v>582</v>
+      </c>
+      <c r="B335" t="s">
         <v>583</v>
-      </c>
-      <c r="B335" t="s">
-        <v>584</v>
       </c>
     </row>
     <row r="336">
       <c r="A336" t="s">
+        <v>584</v>
+      </c>
+      <c r="B336" t="s">
         <v>585</v>
-      </c>
-      <c r="B336" t="s">
-        <v>586</v>
       </c>
     </row>
     <row r="337">
       <c r="A337" t="s">
+        <v>586</v>
+      </c>
+      <c r="B337" t="s">
         <v>587</v>
-      </c>
-      <c r="B337" t="s">
-        <v>588</v>
       </c>
     </row>
     <row r="338">
       <c r="A338" t="s">
+        <v>588</v>
+      </c>
+      <c r="B338" t="s">
         <v>589</v>
-      </c>
-      <c r="B338" t="s">
-        <v>590</v>
       </c>
     </row>
     <row r="339">
       <c r="A339" t="s">
+        <v>590</v>
+      </c>
+      <c r="B339" t="s">
         <v>591</v>
-      </c>
-      <c r="B339" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="340">
@@ -5927,7 +5942,7 @@
         <v>594</v>
       </c>
       <c r="B341" t="s">
-        <v>336</v>
+        <v>313</v>
       </c>
     </row>
     <row r="342">
@@ -5943,23 +5958,23 @@
         <v>597</v>
       </c>
       <c r="B343" t="s">
-        <v>598</v>
+        <v>339</v>
       </c>
     </row>
     <row r="344">
       <c r="A344" t="s">
+        <v>598</v>
+      </c>
+      <c r="B344" t="s">
         <v>599</v>
-      </c>
-      <c r="B344" t="s">
-        <v>600</v>
       </c>
     </row>
     <row r="345">
       <c r="A345" t="s">
+        <v>600</v>
+      </c>
+      <c r="B345" t="s">
         <v>601</v>
-      </c>
-      <c r="B345" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="346">
@@ -5983,7 +5998,7 @@
         <v>606</v>
       </c>
       <c r="B348" t="s">
-        <v>153</v>
+        <v>339</v>
       </c>
     </row>
     <row r="349">
@@ -5991,119 +6006,119 @@
         <v>607</v>
       </c>
       <c r="B349" t="s">
-        <v>127</v>
+        <v>608</v>
       </c>
     </row>
     <row r="350">
       <c r="A350" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="B350" t="s">
-        <v>300</v>
+        <v>610</v>
       </c>
     </row>
     <row r="351">
       <c r="A351" t="s">
-        <v>609</v>
+        <v>611</v>
       </c>
       <c r="B351" t="s">
-        <v>68</v>
+        <v>153</v>
       </c>
     </row>
     <row r="352">
       <c r="A352" t="s">
-        <v>610</v>
+        <v>612</v>
       </c>
       <c r="B352" t="s">
-        <v>611</v>
+        <v>127</v>
       </c>
     </row>
     <row r="353">
       <c r="A353" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="B353" t="s">
-        <v>222</v>
+        <v>303</v>
       </c>
     </row>
     <row r="354">
       <c r="A354" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="B354" t="s">
-        <v>213</v>
+        <v>68</v>
       </c>
     </row>
     <row r="355">
       <c r="A355" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="B355" t="s">
-        <v>169</v>
+        <v>616</v>
       </c>
     </row>
     <row r="356">
       <c r="A356" t="s">
-        <v>615</v>
+        <v>617</v>
       </c>
       <c r="B356" t="s">
-        <v>332</v>
+        <v>225</v>
       </c>
     </row>
     <row r="357">
       <c r="A357" t="s">
-        <v>616</v>
+        <v>618</v>
       </c>
       <c r="B357" t="s">
-        <v>617</v>
+        <v>216</v>
       </c>
     </row>
     <row r="358">
       <c r="A358" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="B358" t="s">
-        <v>483</v>
+        <v>169</v>
       </c>
     </row>
     <row r="359">
       <c r="A359" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="B359" t="s">
-        <v>286</v>
+        <v>335</v>
       </c>
     </row>
     <row r="360">
       <c r="A360" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="B360" t="s">
-        <v>282</v>
+        <v>622</v>
       </c>
     </row>
     <row r="361">
       <c r="A361" t="s">
-        <v>621</v>
+        <v>623</v>
       </c>
       <c r="B361" t="s">
-        <v>622</v>
+        <v>486</v>
       </c>
     </row>
     <row r="362">
       <c r="A362" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="B362" t="s">
-        <v>336</v>
+        <v>289</v>
       </c>
     </row>
     <row r="363">
       <c r="A363" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="B363" t="s">
-        <v>625</v>
+        <v>285</v>
       </c>
     </row>
     <row r="364">
@@ -6119,23 +6134,23 @@
         <v>628</v>
       </c>
       <c r="B365" t="s">
-        <v>629</v>
+        <v>339</v>
       </c>
     </row>
     <row r="366">
       <c r="A366" t="s">
+        <v>629</v>
+      </c>
+      <c r="B366" t="s">
         <v>630</v>
-      </c>
-      <c r="B366" t="s">
-        <v>631</v>
       </c>
     </row>
     <row r="367">
       <c r="A367" t="s">
+        <v>631</v>
+      </c>
+      <c r="B367" t="s">
         <v>632</v>
-      </c>
-      <c r="B367" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="368">
@@ -6143,23 +6158,23 @@
         <v>633</v>
       </c>
       <c r="B368" t="s">
-        <v>251</v>
+        <v>634</v>
       </c>
     </row>
     <row r="369">
       <c r="A369" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="B369" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
     </row>
     <row r="370">
       <c r="A370" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="B370" t="s">
-        <v>637</v>
+        <v>99</v>
       </c>
     </row>
     <row r="371">
@@ -6167,47 +6182,47 @@
         <v>638</v>
       </c>
       <c r="B371" t="s">
-        <v>639</v>
+        <v>254</v>
       </c>
     </row>
     <row r="372">
       <c r="A372" t="s">
+        <v>639</v>
+      </c>
+      <c r="B372" t="s">
         <v>640</v>
-      </c>
-      <c r="B372" t="s">
-        <v>641</v>
       </c>
     </row>
     <row r="373">
       <c r="A373" t="s">
+        <v>641</v>
+      </c>
+      <c r="B373" t="s">
         <v>642</v>
-      </c>
-      <c r="B373" t="s">
-        <v>643</v>
       </c>
     </row>
     <row r="374">
       <c r="A374" t="s">
+        <v>643</v>
+      </c>
+      <c r="B374" t="s">
         <v>644</v>
-      </c>
-      <c r="B374" t="s">
-        <v>645</v>
       </c>
     </row>
     <row r="375">
       <c r="A375" t="s">
+        <v>645</v>
+      </c>
+      <c r="B375" t="s">
         <v>646</v>
-      </c>
-      <c r="B375" t="s">
-        <v>647</v>
       </c>
     </row>
     <row r="376">
       <c r="A376" t="s">
+        <v>647</v>
+      </c>
+      <c r="B376" t="s">
         <v>648</v>
-      </c>
-      <c r="B376" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="377">
@@ -6215,31 +6230,31 @@
         <v>649</v>
       </c>
       <c r="B377" t="s">
-        <v>75</v>
+        <v>650</v>
       </c>
     </row>
     <row r="378">
       <c r="A378" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="B378" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
     </row>
     <row r="379">
       <c r="A379" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="B379" t="s">
-        <v>310</v>
+        <v>227</v>
       </c>
     </row>
     <row r="380">
       <c r="A380" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="B380" t="s">
-        <v>654</v>
+        <v>75</v>
       </c>
     </row>
     <row r="381">
@@ -6247,39 +6262,39 @@
         <v>655</v>
       </c>
       <c r="B381" t="s">
-        <v>443</v>
+        <v>656</v>
       </c>
     </row>
     <row r="382">
       <c r="A382" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="B382" t="s">
-        <v>205</v>
+        <v>313</v>
       </c>
     </row>
     <row r="383">
       <c r="A383" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="B383" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
     </row>
     <row r="384">
       <c r="A384" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="B384" t="s">
-        <v>239</v>
+        <v>446</v>
       </c>
     </row>
     <row r="385">
       <c r="A385" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="B385" t="s">
-        <v>661</v>
+        <v>208</v>
       </c>
     </row>
     <row r="386">
@@ -6295,7 +6310,7 @@
         <v>664</v>
       </c>
       <c r="B387" t="s">
-        <v>111</v>
+        <v>242</v>
       </c>
     </row>
     <row r="388">
@@ -6311,15 +6326,15 @@
         <v>667</v>
       </c>
       <c r="B389" t="s">
-        <v>310</v>
+        <v>668</v>
       </c>
     </row>
     <row r="390">
       <c r="A390" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="B390" t="s">
-        <v>669</v>
+        <v>111</v>
       </c>
     </row>
     <row r="391">
@@ -6327,47 +6342,47 @@
         <v>670</v>
       </c>
       <c r="B391" t="s">
-        <v>171</v>
+        <v>671</v>
       </c>
     </row>
     <row r="392">
       <c r="A392" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="B392" t="s">
-        <v>220</v>
+        <v>313</v>
       </c>
     </row>
     <row r="393">
       <c r="A393" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="B393" t="s">
-        <v>526</v>
+        <v>674</v>
       </c>
     </row>
     <row r="394">
       <c r="A394" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="B394" t="s">
-        <v>674</v>
+        <v>171</v>
       </c>
     </row>
     <row r="395">
       <c r="A395" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="B395" t="s">
-        <v>193</v>
+        <v>223</v>
       </c>
     </row>
     <row r="396">
       <c r="A396" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="B396" t="s">
-        <v>677</v>
+        <v>529</v>
       </c>
     </row>
     <row r="397">
@@ -6383,15 +6398,15 @@
         <v>680</v>
       </c>
       <c r="B398" t="s">
-        <v>681</v>
+        <v>193</v>
       </c>
     </row>
     <row r="399">
       <c r="A399" t="s">
+        <v>681</v>
+      </c>
+      <c r="B399" t="s">
         <v>682</v>
-      </c>
-      <c r="B399" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="400">
@@ -6399,23 +6414,23 @@
         <v>683</v>
       </c>
       <c r="B400" t="s">
-        <v>459</v>
+        <v>684</v>
       </c>
     </row>
     <row r="401">
       <c r="A401" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="B401" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
     </row>
     <row r="402">
       <c r="A402" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="B402" t="s">
-        <v>687</v>
+        <v>153</v>
       </c>
     </row>
     <row r="403">
@@ -6423,7 +6438,7 @@
         <v>688</v>
       </c>
       <c r="B403" t="s">
-        <v>75</v>
+        <v>462</v>
       </c>
     </row>
     <row r="404">
@@ -6431,31 +6446,31 @@
         <v>689</v>
       </c>
       <c r="B404" t="s">
-        <v>327</v>
+        <v>690</v>
       </c>
     </row>
     <row r="405">
       <c r="A405" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="B405" t="s">
-        <v>34</v>
+        <v>692</v>
       </c>
     </row>
     <row r="406">
       <c r="A406" t="s">
-        <v>691</v>
+        <v>693</v>
       </c>
       <c r="B406" t="s">
-        <v>692</v>
+        <v>75</v>
       </c>
     </row>
     <row r="407">
       <c r="A407" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="B407" t="s">
-        <v>694</v>
+        <v>330</v>
       </c>
     </row>
     <row r="408">
@@ -6463,7 +6478,7 @@
         <v>695</v>
       </c>
       <c r="B408" t="s">
-        <v>111</v>
+        <v>34</v>
       </c>
     </row>
     <row r="409">
@@ -6471,23 +6486,23 @@
         <v>696</v>
       </c>
       <c r="B409" t="s">
-        <v>339</v>
+        <v>697</v>
       </c>
     </row>
     <row r="410">
       <c r="A410" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="B410" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
     </row>
     <row r="411">
       <c r="A411" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="B411" t="s">
-        <v>700</v>
+        <v>111</v>
       </c>
     </row>
     <row r="412">
@@ -6495,7 +6510,7 @@
         <v>701</v>
       </c>
       <c r="B412" t="s">
-        <v>306</v>
+        <v>342</v>
       </c>
     </row>
     <row r="413">
@@ -6511,15 +6526,15 @@
         <v>704</v>
       </c>
       <c r="B414" t="s">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="415">
       <c r="A415" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="B415" t="s">
-        <v>706</v>
+        <v>309</v>
       </c>
     </row>
     <row r="416">
@@ -6527,15 +6542,15 @@
         <v>707</v>
       </c>
       <c r="B416" t="s">
-        <v>476</v>
+        <v>708</v>
       </c>
     </row>
     <row r="417">
       <c r="A417" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="B417" t="s">
-        <v>709</v>
+        <v>705</v>
       </c>
     </row>
     <row r="418">
@@ -6543,55 +6558,55 @@
         <v>710</v>
       </c>
       <c r="B418" t="s">
-        <v>88</v>
+        <v>711</v>
       </c>
     </row>
     <row r="419">
       <c r="A419" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="B419" t="s">
-        <v>316</v>
+        <v>479</v>
       </c>
     </row>
     <row r="420">
       <c r="A420" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="B420" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
     </row>
     <row r="421">
       <c r="A421" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="B421" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
     </row>
     <row r="422">
       <c r="A422" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="B422" t="s">
-        <v>127</v>
+        <v>319</v>
       </c>
     </row>
     <row r="423">
       <c r="A423" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="B423" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
     </row>
     <row r="424">
       <c r="A424" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="B424" t="s">
-        <v>719</v>
+        <v>101</v>
       </c>
     </row>
     <row r="425">
@@ -6599,7 +6614,7 @@
         <v>720</v>
       </c>
       <c r="B425" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="426">
@@ -6607,23 +6622,23 @@
         <v>721</v>
       </c>
       <c r="B426" t="s">
-        <v>111</v>
+        <v>722</v>
       </c>
     </row>
     <row r="427">
       <c r="A427" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="B427" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
     </row>
     <row r="428">
       <c r="A428" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="B428" t="s">
-        <v>725</v>
+        <v>117</v>
       </c>
     </row>
     <row r="429">
@@ -6631,239 +6646,263 @@
         <v>726</v>
       </c>
       <c r="B429" t="s">
-        <v>727</v>
+        <v>111</v>
       </c>
     </row>
     <row r="430">
       <c r="A430" t="s">
+        <v>727</v>
+      </c>
+      <c r="B430" t="s">
         <v>728</v>
-      </c>
-      <c r="B430" t="s">
-        <v>729</v>
       </c>
     </row>
     <row r="431">
       <c r="A431" t="s">
+        <v>729</v>
+      </c>
+      <c r="B431" t="s">
         <v>730</v>
-      </c>
-      <c r="B431" t="s">
-        <v>731</v>
       </c>
     </row>
     <row r="432">
       <c r="A432" t="s">
-        <v>93</v>
+        <v>731</v>
       </c>
       <c r="B432" t="s">
-        <v>94</v>
+        <v>732</v>
       </c>
     </row>
     <row r="433">
       <c r="A433" t="s">
-        <v>104</v>
+        <v>733</v>
       </c>
       <c r="B433" t="s">
-        <v>732</v>
+        <v>734</v>
       </c>
     </row>
     <row r="434">
       <c r="A434" t="s">
-        <v>733</v>
+        <v>735</v>
       </c>
       <c r="B434" t="s">
-        <v>734</v>
+        <v>736</v>
       </c>
     </row>
     <row r="435">
       <c r="A435" t="s">
-        <v>735</v>
+        <v>93</v>
       </c>
       <c r="B435" t="s">
-        <v>729</v>
+        <v>94</v>
       </c>
     </row>
     <row r="436">
       <c r="A436" t="s">
-        <v>736</v>
+        <v>104</v>
       </c>
       <c r="B436" t="s">
-        <v>729</v>
+        <v>737</v>
       </c>
     </row>
     <row r="437">
       <c r="A437" t="s">
-        <v>214</v>
+        <v>738</v>
       </c>
       <c r="B437" t="s">
-        <v>215</v>
+        <v>739</v>
       </c>
     </row>
     <row r="438">
       <c r="A438" t="s">
-        <v>737</v>
+        <v>740</v>
       </c>
       <c r="B438" t="s">
-        <v>729</v>
+        <v>734</v>
       </c>
     </row>
     <row r="439">
       <c r="A439" t="s">
-        <v>738</v>
+        <v>741</v>
       </c>
       <c r="B439" t="s">
-        <v>729</v>
+        <v>734</v>
       </c>
     </row>
     <row r="440">
       <c r="A440" t="s">
-        <v>739</v>
+        <v>217</v>
       </c>
       <c r="B440" t="s">
-        <v>729</v>
+        <v>218</v>
       </c>
     </row>
     <row r="441">
       <c r="A441" t="s">
-        <v>740</v>
+        <v>742</v>
       </c>
       <c r="B441" t="s">
-        <v>741</v>
+        <v>734</v>
       </c>
     </row>
     <row r="442">
       <c r="A442" t="s">
-        <v>367</v>
+        <v>743</v>
       </c>
       <c r="B442" t="s">
-        <v>368</v>
+        <v>734</v>
       </c>
     </row>
     <row r="443">
       <c r="A443" t="s">
-        <v>406</v>
+        <v>744</v>
       </c>
       <c r="B443" t="s">
-        <v>407</v>
+        <v>734</v>
       </c>
     </row>
     <row r="444">
       <c r="A444" t="s">
-        <v>408</v>
+        <v>745</v>
       </c>
       <c r="B444" t="s">
-        <v>409</v>
+        <v>746</v>
       </c>
     </row>
     <row r="445">
       <c r="A445" t="s">
-        <v>742</v>
+        <v>370</v>
       </c>
       <c r="B445" t="s">
-        <v>729</v>
+        <v>371</v>
       </c>
     </row>
     <row r="446">
       <c r="A446" t="s">
-        <v>417</v>
+        <v>409</v>
       </c>
       <c r="B446" t="s">
-        <v>418</v>
+        <v>410</v>
       </c>
     </row>
     <row r="447">
       <c r="A447" t="s">
-        <v>435</v>
+        <v>411</v>
       </c>
       <c r="B447" t="s">
-        <v>743</v>
+        <v>412</v>
       </c>
     </row>
     <row r="448">
       <c r="A448" t="s">
-        <v>440</v>
+        <v>747</v>
       </c>
       <c r="B448" t="s">
-        <v>441</v>
+        <v>734</v>
       </c>
     </row>
     <row r="449">
       <c r="A449" t="s">
-        <v>744</v>
+        <v>420</v>
       </c>
       <c r="B449" t="s">
-        <v>729</v>
+        <v>421</v>
       </c>
     </row>
     <row r="450">
       <c r="A450" t="s">
-        <v>579</v>
+        <v>438</v>
       </c>
       <c r="B450" t="s">
-        <v>580</v>
+        <v>748</v>
       </c>
     </row>
     <row r="451">
       <c r="A451" t="s">
-        <v>636</v>
+        <v>443</v>
       </c>
       <c r="B451" t="s">
-        <v>637</v>
+        <v>444</v>
       </c>
     </row>
     <row r="452">
       <c r="A452" t="s">
-        <v>745</v>
+        <v>749</v>
       </c>
       <c r="B452" t="s">
-        <v>729</v>
+        <v>734</v>
       </c>
     </row>
     <row r="453">
       <c r="A453" t="s">
-        <v>746</v>
+        <v>582</v>
       </c>
       <c r="B453" t="s">
-        <v>729</v>
+        <v>583</v>
       </c>
     </row>
     <row r="454">
       <c r="A454" t="s">
-        <v>747</v>
+        <v>641</v>
       </c>
       <c r="B454" t="s">
-        <v>729</v>
+        <v>642</v>
       </c>
     </row>
     <row r="455">
       <c r="A455" t="s">
-        <v>653</v>
+        <v>750</v>
       </c>
       <c r="B455" t="s">
-        <v>654</v>
+        <v>734</v>
       </c>
     </row>
     <row r="456">
       <c r="A456" t="s">
-        <v>748</v>
+        <v>751</v>
       </c>
       <c r="B456" t="s">
-        <v>729</v>
+        <v>734</v>
       </c>
     </row>
     <row r="457">
       <c r="A457" t="s">
-        <v>749</v>
+        <v>752</v>
       </c>
       <c r="B457" t="s">
-        <v>729</v>
+        <v>734</v>
       </c>
     </row>
     <row r="458">
       <c r="A458" t="s">
-        <v>750</v>
+        <v>658</v>
       </c>
       <c r="B458" t="s">
-        <v>729</v>
+        <v>659</v>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="s">
+        <v>753</v>
+      </c>
+      <c r="B459" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="s">
+        <v>754</v>
+      </c>
+      <c r="B460" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="s">
+        <v>755</v>
+      </c>
+      <c r="B461" t="s">
+        <v>734</v>
       </c>
     </row>
   </sheetData>
@@ -6882,7 +6921,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>751</v>
+        <v>756</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -6890,55 +6929,55 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>752</v>
+        <v>757</v>
       </c>
       <c r="B2" t="s">
-        <v>753</v>
+        <v>758</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>754</v>
+        <v>759</v>
       </c>
       <c r="B3" t="s">
-        <v>755</v>
+        <v>760</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>756</v>
+        <v>761</v>
       </c>
       <c r="B4" t="s">
-        <v>757</v>
+        <v>762</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>758</v>
+        <v>763</v>
       </c>
       <c r="B5" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>759</v>
+        <v>764</v>
       </c>
       <c r="B6" t="s">
-        <v>760</v>
+        <v>765</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>761</v>
+        <v>766</v>
       </c>
       <c r="B7" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>762</v>
+        <v>767</v>
       </c>
       <c r="B8" t="s">
         <v>82</v>
@@ -6946,199 +6985,199 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>763</v>
+        <v>768</v>
       </c>
       <c r="B9" t="s">
-        <v>553</v>
+        <v>556</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>764</v>
+        <v>769</v>
       </c>
       <c r="B10" t="s">
-        <v>765</v>
+        <v>770</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>766</v>
+        <v>771</v>
       </c>
       <c r="B11" t="s">
-        <v>767</v>
+        <v>772</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>768</v>
+        <v>773</v>
       </c>
       <c r="B12" t="s">
-        <v>445</v>
+        <v>448</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>769</v>
+        <v>774</v>
       </c>
       <c r="B13" t="s">
-        <v>770</v>
+        <v>775</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>771</v>
+        <v>776</v>
       </c>
       <c r="B14" t="s">
-        <v>772</v>
+        <v>777</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>773</v>
+        <v>778</v>
       </c>
       <c r="B15" t="s">
-        <v>774</v>
+        <v>779</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>775</v>
+        <v>780</v>
       </c>
       <c r="B16" t="s">
-        <v>776</v>
+        <v>781</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>777</v>
+        <v>782</v>
       </c>
       <c r="B17" t="s">
-        <v>778</v>
+        <v>783</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>779</v>
+        <v>784</v>
       </c>
       <c r="B18" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>780</v>
+        <v>785</v>
       </c>
       <c r="B19" t="s">
-        <v>781</v>
+        <v>786</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>782</v>
+        <v>787</v>
       </c>
       <c r="B20" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>783</v>
+        <v>788</v>
       </c>
       <c r="B21" t="s">
-        <v>784</v>
+        <v>789</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>785</v>
+        <v>790</v>
       </c>
       <c r="B22" t="s">
-        <v>786</v>
+        <v>791</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>787</v>
+        <v>792</v>
       </c>
       <c r="B23" t="s">
-        <v>788</v>
+        <v>793</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>789</v>
+        <v>794</v>
       </c>
       <c r="B24" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>790</v>
+        <v>795</v>
       </c>
       <c r="B25" t="s">
-        <v>791</v>
+        <v>796</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>792</v>
+        <v>797</v>
       </c>
       <c r="B26" t="s">
-        <v>793</v>
+        <v>798</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>794</v>
+        <v>799</v>
       </c>
       <c r="B27" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>795</v>
+        <v>800</v>
       </c>
       <c r="B28" t="s">
-        <v>796</v>
+        <v>801</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>797</v>
+        <v>802</v>
       </c>
       <c r="B29" t="s">
-        <v>798</v>
+        <v>803</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>799</v>
+        <v>804</v>
       </c>
       <c r="B30" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>800</v>
+        <v>805</v>
       </c>
       <c r="B31" t="s">
-        <v>801</v>
+        <v>806</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>802</v>
+        <v>807</v>
       </c>
       <c r="B32" t="s">
-        <v>803</v>
+        <v>808</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>804</v>
+        <v>809</v>
       </c>
       <c r="B33" t="s">
         <v>88</v>
@@ -7146,7 +7185,7 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>805</v>
+        <v>810</v>
       </c>
       <c r="B34" t="s">
         <v>68</v>
@@ -7154,71 +7193,71 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>806</v>
+        <v>811</v>
       </c>
       <c r="B35" t="s">
-        <v>807</v>
+        <v>812</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>808</v>
+        <v>813</v>
       </c>
       <c r="B36" t="s">
-        <v>809</v>
+        <v>814</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>810</v>
+        <v>815</v>
       </c>
       <c r="B37" t="s">
-        <v>811</v>
+        <v>816</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>812</v>
+        <v>817</v>
       </c>
       <c r="B38" t="s">
-        <v>813</v>
+        <v>818</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>814</v>
+        <v>819</v>
       </c>
       <c r="B39" t="s">
-        <v>815</v>
+        <v>820</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>816</v>
+        <v>821</v>
       </c>
       <c r="B40" t="s">
-        <v>817</v>
+        <v>822</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>818</v>
+        <v>823</v>
       </c>
       <c r="B41" t="s">
-        <v>819</v>
+        <v>824</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>820</v>
+        <v>825</v>
       </c>
       <c r="B42" t="s">
-        <v>821</v>
+        <v>826</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>822</v>
+        <v>827</v>
       </c>
       <c r="B43" t="s">
         <v>82</v>
@@ -7226,135 +7265,135 @@
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>823</v>
+        <v>828</v>
       </c>
       <c r="B44" t="s">
-        <v>824</v>
+        <v>829</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>825</v>
+        <v>830</v>
       </c>
       <c r="B45" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>826</v>
+        <v>831</v>
       </c>
       <c r="B46" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>827</v>
+        <v>832</v>
       </c>
       <c r="B47" t="s">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>828</v>
+        <v>833</v>
       </c>
       <c r="B48" t="s">
-        <v>829</v>
+        <v>834</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>830</v>
+        <v>835</v>
       </c>
       <c r="B49" t="s">
-        <v>831</v>
+        <v>836</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>832</v>
+        <v>837</v>
       </c>
       <c r="B50" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>833</v>
+        <v>838</v>
       </c>
       <c r="B51" t="s">
-        <v>834</v>
+        <v>839</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>835</v>
+        <v>840</v>
       </c>
       <c r="B52" t="s">
-        <v>836</v>
+        <v>841</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>837</v>
+        <v>842</v>
       </c>
       <c r="B53" t="s">
-        <v>838</v>
+        <v>843</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>839</v>
+        <v>844</v>
       </c>
       <c r="B54" t="s">
-        <v>840</v>
+        <v>845</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>841</v>
+        <v>846</v>
       </c>
       <c r="B55" t="s">
-        <v>842</v>
+        <v>847</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>843</v>
+        <v>848</v>
       </c>
       <c r="B56" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>844</v>
+        <v>849</v>
       </c>
       <c r="B57" t="s">
-        <v>845</v>
+        <v>850</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>846</v>
+        <v>851</v>
       </c>
       <c r="B58" t="s">
-        <v>847</v>
+        <v>852</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>848</v>
+        <v>853</v>
       </c>
       <c r="B59" t="s">
-        <v>849</v>
+        <v>854</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>850</v>
+        <v>855</v>
       </c>
       <c r="B60" t="s">
         <v>32</v>
@@ -7362,143 +7401,143 @@
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>851</v>
+        <v>856</v>
       </c>
       <c r="B61" t="s">
-        <v>852</v>
+        <v>857</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>853</v>
+        <v>858</v>
       </c>
       <c r="B62" t="s">
-        <v>854</v>
+        <v>859</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>855</v>
+        <v>860</v>
       </c>
       <c r="B63" t="s">
-        <v>847</v>
+        <v>852</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>856</v>
+        <v>861</v>
       </c>
       <c r="B64" t="s">
-        <v>857</v>
+        <v>862</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>858</v>
+        <v>863</v>
       </c>
       <c r="B65" t="s">
-        <v>859</v>
+        <v>864</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>860</v>
+        <v>865</v>
       </c>
       <c r="B66" t="s">
-        <v>861</v>
+        <v>866</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>862</v>
+        <v>867</v>
       </c>
       <c r="B67" t="s">
-        <v>863</v>
+        <v>868</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>864</v>
+        <v>869</v>
       </c>
       <c r="B68" t="s">
-        <v>865</v>
+        <v>870</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>866</v>
+        <v>871</v>
       </c>
       <c r="B69" t="s">
-        <v>867</v>
+        <v>872</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>868</v>
+        <v>873</v>
       </c>
       <c r="B70" t="s">
-        <v>869</v>
+        <v>874</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>870</v>
+        <v>875</v>
       </c>
       <c r="B71" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>871</v>
+        <v>876</v>
       </c>
       <c r="B72" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>872</v>
+        <v>877</v>
       </c>
       <c r="B73" t="s">
-        <v>873</v>
+        <v>878</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>754</v>
+        <v>759</v>
       </c>
       <c r="B74" t="s">
-        <v>755</v>
+        <v>760</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>874</v>
+        <v>879</v>
       </c>
       <c r="B75" t="s">
-        <v>767</v>
+        <v>772</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>875</v>
+        <v>880</v>
       </c>
       <c r="B76" t="s">
-        <v>876</v>
+        <v>881</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>877</v>
+        <v>882</v>
       </c>
       <c r="B77" t="s">
-        <v>878</v>
+        <v>883</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>879</v>
+        <v>884</v>
       </c>
       <c r="B78" t="s">
         <v>171</v>
@@ -7506,71 +7545,71 @@
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>880</v>
+        <v>885</v>
       </c>
       <c r="B79" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>881</v>
+        <v>886</v>
       </c>
       <c r="B80" t="s">
-        <v>882</v>
+        <v>887</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>883</v>
+        <v>888</v>
       </c>
       <c r="B81" t="s">
-        <v>884</v>
+        <v>889</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>885</v>
+        <v>890</v>
       </c>
       <c r="B82" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>886</v>
+        <v>891</v>
       </c>
       <c r="B83" t="s">
-        <v>887</v>
+        <v>892</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>888</v>
+        <v>893</v>
       </c>
       <c r="B84" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>889</v>
+        <v>894</v>
       </c>
       <c r="B85" t="s">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>890</v>
+        <v>895</v>
       </c>
       <c r="B86" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>891</v>
+        <v>896</v>
       </c>
       <c r="B87" t="s">
         <v>17</v>
@@ -7578,7 +7617,7 @@
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>892</v>
+        <v>897</v>
       </c>
       <c r="B88" t="s">
         <v>101</v>
@@ -7600,68 +7639,68 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>751</v>
+        <v>756</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>893</v>
+        <v>898</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>894</v>
+        <v>899</v>
       </c>
       <c r="B2" t="s">
-        <v>895</v>
+        <v>900</v>
       </c>
       <c r="C2" t="s">
-        <v>896</v>
+        <v>901</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>897</v>
+        <v>902</v>
       </c>
       <c r="B3" t="s">
-        <v>898</v>
+        <v>903</v>
       </c>
       <c r="C3" t="s">
-        <v>899</v>
+        <v>904</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>900</v>
+        <v>905</v>
       </c>
       <c r="B4" t="s">
-        <v>901</v>
+        <v>906</v>
       </c>
       <c r="C4" t="s">
-        <v>902</v>
+        <v>907</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>903</v>
+        <v>908</v>
       </c>
       <c r="B5" t="s">
-        <v>904</v>
+        <v>909</v>
       </c>
       <c r="C5" t="s">
-        <v>905</v>
+        <v>910</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>906</v>
+        <v>911</v>
       </c>
       <c r="B6" t="s">
-        <v>907</v>
+        <v>912</v>
       </c>
       <c r="C6" t="s">
-        <v>908</v>
+        <v>913</v>
       </c>
     </row>
   </sheetData>
@@ -7680,233 +7719,233 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>751</v>
+        <v>756</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>909</v>
+        <v>914</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>910</v>
+        <v>915</v>
       </c>
       <c r="B2" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="C2" t="s">
-        <v>911</v>
+        <v>916</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>912</v>
+        <v>917</v>
       </c>
       <c r="B3" t="s">
-        <v>913</v>
+        <v>918</v>
       </c>
       <c r="C3" t="s">
-        <v>914</v>
+        <v>919</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>915</v>
+        <v>920</v>
       </c>
       <c r="B4" t="s">
-        <v>916</v>
+        <v>921</v>
       </c>
       <c r="C4" t="s">
-        <v>914</v>
+        <v>919</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>917</v>
+        <v>922</v>
       </c>
       <c r="B5" t="s">
-        <v>867</v>
+        <v>872</v>
       </c>
       <c r="C5" t="s">
-        <v>918</v>
+        <v>923</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>919</v>
+        <v>924</v>
       </c>
       <c r="B6" t="s">
-        <v>920</v>
+        <v>925</v>
       </c>
       <c r="C6" t="s">
-        <v>918</v>
+        <v>923</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>921</v>
+        <v>926</v>
       </c>
       <c r="B7" t="s">
         <v>75</v>
       </c>
       <c r="C7" t="s">
-        <v>922</v>
+        <v>927</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>923</v>
+        <v>928</v>
       </c>
       <c r="B8" t="s">
-        <v>924</v>
+        <v>929</v>
       </c>
       <c r="C8" t="s">
-        <v>925</v>
+        <v>930</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>926</v>
+        <v>931</v>
       </c>
       <c r="B9" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C9" t="s">
-        <v>925</v>
+        <v>930</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>927</v>
+        <v>932</v>
       </c>
       <c r="B10" t="s">
-        <v>873</v>
+        <v>878</v>
       </c>
       <c r="C10" t="s">
-        <v>925</v>
+        <v>930</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>928</v>
+        <v>933</v>
       </c>
       <c r="B11" t="s">
         <v>88</v>
       </c>
       <c r="C11" t="s">
-        <v>925</v>
+        <v>930</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>929</v>
+        <v>934</v>
       </c>
       <c r="B12" t="s">
-        <v>930</v>
+        <v>935</v>
       </c>
       <c r="C12" t="s">
-        <v>931</v>
+        <v>936</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>932</v>
+        <v>937</v>
       </c>
       <c r="B13" t="s">
-        <v>933</v>
+        <v>938</v>
       </c>
       <c r="C13" t="s">
-        <v>934</v>
+        <v>939</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>935</v>
+        <v>940</v>
       </c>
       <c r="B14" t="s">
+        <v>941</v>
+      </c>
+      <c r="C14" t="s">
         <v>936</v>
-      </c>
-      <c r="C14" t="s">
-        <v>931</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>937</v>
+        <v>942</v>
       </c>
       <c r="B15" t="s">
         <v>38</v>
       </c>
       <c r="C15" t="s">
-        <v>938</v>
+        <v>943</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>939</v>
+        <v>944</v>
       </c>
       <c r="B16" t="s">
         <v>68</v>
       </c>
       <c r="C16" t="s">
-        <v>940</v>
+        <v>945</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>935</v>
+        <v>940</v>
       </c>
       <c r="B17" t="s">
-        <v>941</v>
+        <v>946</v>
       </c>
       <c r="C17" t="s">
-        <v>942</v>
+        <v>947</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>943</v>
+        <v>948</v>
       </c>
       <c r="B18" t="s">
-        <v>944</v>
+        <v>949</v>
       </c>
       <c r="C18" t="s">
-        <v>945</v>
+        <v>950</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>946</v>
+        <v>951</v>
       </c>
       <c r="B19" t="s">
-        <v>947</v>
+        <v>952</v>
       </c>
       <c r="C19" t="s">
-        <v>948</v>
+        <v>953</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>949</v>
+        <v>954</v>
       </c>
       <c r="B20" t="s">
         <v>115</v>
       </c>
       <c r="C20" t="s">
-        <v>948</v>
+        <v>953</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>950</v>
+        <v>955</v>
       </c>
       <c r="B21" t="s">
-        <v>907</v>
+        <v>912</v>
       </c>
       <c r="C21" t="s">
-        <v>951</v>
+        <v>956</v>
       </c>
     </row>
   </sheetData>

</xml_diff>